<commit_message>
Update to assess missing countries
</commit_message>
<xml_diff>
--- a/research/cross_crisis/indecies_crisis_definitions_comparison.xlsx
+++ b/research/cross_crisis/indecies_crisis_definitions_comparison.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\IMF_VE_News\research\cross_crisis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{A7EBA77D-8BA5-4EC6-8107-C9D528082BCC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE6A51F1-B871-429C-9571-D729084A1FA8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cross_comparison" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="30">
   <si>
     <t>LoDuca</t>
   </si>
@@ -95,12 +95,27 @@
   </si>
   <si>
     <t>Evaluation of Indecies' Signals Against Different Events/Crisis Definitions</t>
+  </si>
+  <si>
+    <t>IMF Program Requests (Monthly precision)</t>
+  </si>
+  <si>
+    <t>NOTE: Not all countries - only those included in the 'Fund Arrangements since 1952 updated_0612.xlsx' file</t>
+  </si>
+  <si>
+    <t>All Program Starts</t>
+  </si>
+  <si>
+    <t>All Program Starts - Gap 3 Years</t>
+  </si>
+  <si>
+    <t>All Program Starts - Gap 6 Years</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -244,7 +259,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -427,6 +442,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -609,29 +630,31 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -986,11 +1009,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AE17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AE24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1014,149 +1037,149 @@
       </c>
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="4" t="s">
+      <c r="C5" s="14"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="5"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="4" t="s">
+      <c r="F5" s="14"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="I5" s="5"/>
-      <c r="J5" s="12"/>
-      <c r="K5" s="4" t="s">
+      <c r="I5" s="14"/>
+      <c r="J5" s="15"/>
+      <c r="K5" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="L5" s="5"/>
-      <c r="M5" s="12"/>
-      <c r="N5" s="4" t="s">
+      <c r="L5" s="14"/>
+      <c r="M5" s="15"/>
+      <c r="N5" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="O5" s="5"/>
-      <c r="P5" s="12"/>
-      <c r="Q5" s="4" t="s">
+      <c r="O5" s="14"/>
+      <c r="P5" s="15"/>
+      <c r="Q5" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="R5" s="5"/>
-      <c r="S5" s="12"/>
-      <c r="T5" s="4" t="s">
+      <c r="R5" s="14"/>
+      <c r="S5" s="15"/>
+      <c r="T5" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="U5" s="5"/>
-      <c r="V5" s="12"/>
-      <c r="W5" s="4" t="s">
+      <c r="U5" s="14"/>
+      <c r="V5" s="15"/>
+      <c r="W5" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="X5" s="5"/>
-      <c r="Y5" s="12"/>
-      <c r="Z5" s="4" t="s">
+      <c r="X5" s="14"/>
+      <c r="Y5" s="15"/>
+      <c r="Z5" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="AA5" s="5"/>
-      <c r="AB5" s="12"/>
-      <c r="AC5" s="4" t="s">
+      <c r="AA5" s="14"/>
+      <c r="AB5" s="15"/>
+      <c r="AC5" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="AD5" s="5"/>
-      <c r="AE5" s="12"/>
+      <c r="AD5" s="14"/>
+      <c r="AE5" s="15"/>
     </row>
     <row r="6" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="G6" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="H6" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="I6" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="J6" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="K6" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="L6" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="M6" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="N6" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="O6" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="P6" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q6" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="R6" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="S6" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="T6" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="U6" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="V6" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="W6" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="X6" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="Y6" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="Z6" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="AA6" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="AB6" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="AC6" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="AD6" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="AE6" s="13" t="s">
+      <c r="B6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J6" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="L6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="M6" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="N6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="O6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="P6" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="R6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="S6" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="T6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="U6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="V6" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="W6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="X6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y6" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="AA6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="AB6" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AC6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="AD6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="AE6" s="10" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1164,129 +1187,129 @@
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="8"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="8"/>
-      <c r="I7" s="9"/>
-      <c r="J7" s="14"/>
-      <c r="K7" s="8"/>
-      <c r="L7" s="9"/>
-      <c r="M7" s="14"/>
-      <c r="N7" s="8"/>
-      <c r="O7" s="9"/>
-      <c r="P7" s="14"/>
-      <c r="Q7" s="8"/>
-      <c r="R7" s="9"/>
-      <c r="S7" s="14"/>
-      <c r="T7" s="8"/>
-      <c r="U7" s="9"/>
-      <c r="V7" s="14"/>
-      <c r="W7" s="8"/>
-      <c r="X7" s="9"/>
-      <c r="Y7" s="14"/>
-      <c r="Z7" s="8"/>
-      <c r="AA7" s="9"/>
-      <c r="AB7" s="14"/>
-      <c r="AC7" s="8"/>
-      <c r="AD7" s="9"/>
-      <c r="AE7" s="14"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="11"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="11"/>
+      <c r="N7" s="6"/>
+      <c r="O7" s="7"/>
+      <c r="P7" s="11"/>
+      <c r="Q7" s="6"/>
+      <c r="R7" s="7"/>
+      <c r="S7" s="11"/>
+      <c r="T7" s="6"/>
+      <c r="U7" s="7"/>
+      <c r="V7" s="11"/>
+      <c r="W7" s="6"/>
+      <c r="X7" s="7"/>
+      <c r="Y7" s="11"/>
+      <c r="Z7" s="6"/>
+      <c r="AA7" s="7"/>
+      <c r="AB7" s="11"/>
+      <c r="AC7" s="6"/>
+      <c r="AD7" s="7"/>
+      <c r="AE7" s="11"/>
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="10">
+      <c r="B8" s="8">
         <v>0.82352941176470495</v>
       </c>
-      <c r="C8" s="11">
+      <c r="C8" s="9">
         <v>0.15384615384615299</v>
       </c>
-      <c r="D8" s="15">
+      <c r="D8" s="12">
         <v>0.44025157232704398</v>
       </c>
-      <c r="E8" s="10">
+      <c r="E8" s="8">
         <v>0.83606557377049096</v>
       </c>
-      <c r="F8" s="11">
+      <c r="F8" s="9">
         <v>0.17346938775510201</v>
       </c>
-      <c r="G8" s="15">
+      <c r="G8" s="12">
         <v>0.473977695167286</v>
       </c>
-      <c r="H8" s="10">
+      <c r="H8" s="8">
         <v>0.83673469387755095</v>
       </c>
-      <c r="I8" s="11">
+      <c r="I8" s="9">
         <v>0.18222222222222201</v>
       </c>
-      <c r="J8" s="15">
+      <c r="J8" s="12">
         <v>0.48693586698337199</v>
       </c>
-      <c r="K8" s="10">
+      <c r="K8" s="8">
         <v>0.890625</v>
       </c>
-      <c r="L8" s="11">
+      <c r="L8" s="9">
         <v>0.20577617328519801</v>
       </c>
-      <c r="M8" s="15">
+      <c r="M8" s="12">
         <v>0.53470919324577804</v>
       </c>
-      <c r="N8" s="10">
+      <c r="N8" s="8">
         <v>0.85</v>
       </c>
-      <c r="O8" s="11">
+      <c r="O8" s="9">
         <v>0.155963302752293</v>
       </c>
-      <c r="P8" s="15">
+      <c r="P8" s="12">
         <v>0.44973544973544899</v>
       </c>
-      <c r="Q8" s="10">
+      <c r="Q8" s="8">
         <v>0.81818181818181801</v>
       </c>
-      <c r="R8" s="11">
+      <c r="R8" s="9">
         <v>0.197368421052631</v>
       </c>
-      <c r="S8" s="15">
+      <c r="S8" s="12">
         <v>0.50223214285714202</v>
       </c>
-      <c r="T8" s="10">
+      <c r="T8" s="8">
         <v>0.88524590163934402</v>
       </c>
-      <c r="U8" s="11">
+      <c r="U8" s="9">
         <v>0.21686746987951799</v>
       </c>
-      <c r="V8" s="15">
+      <c r="V8" s="12">
         <v>0.54766734279918805</v>
       </c>
-      <c r="W8" s="10">
+      <c r="W8" s="8">
         <v>0.82142857142857095</v>
       </c>
-      <c r="X8" s="11">
+      <c r="X8" s="9">
         <v>0.206278026905829</v>
       </c>
-      <c r="Y8" s="15">
+      <c r="Y8" s="12">
         <v>0.51454138702460805</v>
       </c>
-      <c r="Z8" s="10">
+      <c r="Z8" s="8">
         <v>0.82758620689655105</v>
       </c>
-      <c r="AA8" s="11">
+      <c r="AA8" s="9">
         <v>0.218181818181818</v>
       </c>
-      <c r="AB8" s="15">
+      <c r="AB8" s="12">
         <v>0.53097345132743301</v>
       </c>
-      <c r="AC8" s="10">
+      <c r="AC8" s="8">
         <v>0.82142857142857095</v>
       </c>
-      <c r="AD8" s="11">
+      <c r="AD8" s="9">
         <v>0.20720720720720701</v>
       </c>
-      <c r="AE8" s="15">
+      <c r="AE8" s="12">
         <v>0.51569506726457304</v>
       </c>
     </row>
@@ -1294,94 +1317,94 @@
       <c r="A9" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="10">
+      <c r="B9" s="8">
         <v>0.82795698924731098</v>
       </c>
-      <c r="C9" s="11">
+      <c r="C9" s="9">
         <v>0.124394184168012</v>
       </c>
-      <c r="D9" s="15">
+      <c r="D9" s="12">
         <v>0.38849646821392497</v>
       </c>
-      <c r="E9" s="10">
+      <c r="E9" s="8">
         <v>0.87</v>
       </c>
-      <c r="F9" s="11">
+      <c r="F9" s="9">
         <v>0.14671163575042101</v>
       </c>
-      <c r="G9" s="15">
+      <c r="G9" s="12">
         <v>0.43806646525679699</v>
       </c>
-      <c r="H9" s="10">
+      <c r="H9" s="8">
         <v>0.80851063829787195</v>
       </c>
-      <c r="I9" s="11">
+      <c r="I9" s="9">
         <v>0.13171577123050199</v>
       </c>
-      <c r="J9" s="15">
+      <c r="J9" s="12">
         <v>0.39874081846799497</v>
       </c>
-      <c r="K9" s="10">
+      <c r="K9" s="8">
         <v>0.82291666666666596</v>
       </c>
-      <c r="L9" s="11">
+      <c r="L9" s="9">
         <v>0.129296235679214</v>
       </c>
-      <c r="M9" s="15">
+      <c r="M9" s="12">
         <v>0.39698492462311502</v>
       </c>
-      <c r="N9" s="10">
+      <c r="N9" s="8">
         <v>0.93617021276595702</v>
       </c>
-      <c r="O9" s="11">
+      <c r="O9" s="9">
         <v>0.189928057553956</v>
       </c>
-      <c r="P9" s="15">
+      <c r="P9" s="12">
         <v>0.52422557585385199</v>
       </c>
-      <c r="Q9" s="10">
+      <c r="Q9" s="8">
         <v>0.88785046728971895</v>
       </c>
-      <c r="R9" s="11">
+      <c r="R9" s="9">
         <v>0.16521739130434701</v>
       </c>
-      <c r="S9" s="15">
+      <c r="S9" s="12">
         <v>0.47357926221336</v>
       </c>
-      <c r="T9" s="10">
+      <c r="T9" s="8">
         <v>0.82291666666666596</v>
       </c>
-      <c r="U9" s="11">
+      <c r="U9" s="9">
         <v>0.143375680580762</v>
       </c>
-      <c r="V9" s="15">
+      <c r="V9" s="12">
         <v>0.42245989304812798</v>
       </c>
-      <c r="W9" s="10">
+      <c r="W9" s="8">
         <v>0.83673469387755095</v>
       </c>
-      <c r="X9" s="11">
+      <c r="X9" s="9">
         <v>0.14260869565217299</v>
       </c>
-      <c r="Y9" s="15">
+      <c r="Y9" s="12">
         <v>0.42399172699069199</v>
       </c>
-      <c r="Z9" s="10">
+      <c r="Z9" s="8">
         <v>0.80434782608695599</v>
       </c>
-      <c r="AA9" s="11">
+      <c r="AA9" s="9">
         <v>0.13653136531365301</v>
       </c>
-      <c r="AB9" s="15">
+      <c r="AB9" s="12">
         <v>0.40659340659340598</v>
       </c>
-      <c r="AC9" s="10">
+      <c r="AC9" s="8">
         <v>0.79569892473118198</v>
       </c>
-      <c r="AD9" s="11">
+      <c r="AD9" s="9">
         <v>0.13805970149253699</v>
       </c>
-      <c r="AE9" s="15">
+      <c r="AE9" s="12">
         <v>0.40748898678413997</v>
       </c>
     </row>
@@ -1389,94 +1412,94 @@
       <c r="A10" t="s">
         <v>1</v>
       </c>
-      <c r="B10" s="10">
+      <c r="B10" s="8">
         <v>0.88235294117647001</v>
       </c>
-      <c r="C10" s="11">
+      <c r="C10" s="9">
         <v>0.13837638376383701</v>
       </c>
-      <c r="D10" s="15">
+      <c r="D10" s="12">
         <v>0.42517006802721002</v>
       </c>
-      <c r="E10" s="10">
+      <c r="E10" s="8">
         <v>0.91397849462365599</v>
       </c>
-      <c r="F10" s="11">
+      <c r="F10" s="9">
         <v>0.155963302752293</v>
       </c>
-      <c r="G10" s="15">
+      <c r="G10" s="12">
         <v>0.46346782988004298</v>
       </c>
-      <c r="H10" s="10">
+      <c r="H10" s="8">
         <v>0.88095238095238004</v>
       </c>
-      <c r="I10" s="11">
+      <c r="I10" s="9">
         <v>0.145669291338582</v>
       </c>
-      <c r="J10" s="15">
+      <c r="J10" s="12">
         <v>0.43838862559241598</v>
       </c>
-      <c r="K10" s="10">
+      <c r="K10" s="8">
         <v>0.89024390243902396</v>
       </c>
-      <c r="L10" s="11">
+      <c r="L10" s="9">
         <v>0.139047619047619</v>
       </c>
-      <c r="M10" s="15">
+      <c r="M10" s="12">
         <v>0.427901524032825</v>
       </c>
-      <c r="N10" s="10">
+      <c r="N10" s="8">
         <v>0.94656488549618301</v>
       </c>
-      <c r="O10" s="11">
+      <c r="O10" s="9">
         <v>0.20945945945945901</v>
       </c>
-      <c r="P10" s="15">
+      <c r="P10" s="12">
         <v>0.55555555555555503</v>
       </c>
-      <c r="Q10" s="10">
+      <c r="Q10" s="8">
         <v>0.89772727272727204</v>
       </c>
-      <c r="R10" s="11">
+      <c r="R10" s="9">
         <v>0.15895372233400301</v>
       </c>
-      <c r="S10" s="15">
+      <c r="S10" s="12">
         <v>0.46525323910482902</v>
       </c>
-      <c r="T10" s="10">
+      <c r="T10" s="8">
         <v>0.89772727272727204</v>
       </c>
-      <c r="U10" s="11">
+      <c r="U10" s="9">
         <v>0.15863453815261</v>
       </c>
-      <c r="V10" s="15">
+      <c r="V10" s="12">
         <v>0.46470588235294102</v>
       </c>
-      <c r="W10" s="10">
+      <c r="W10" s="8">
         <v>0.87804878048780399</v>
       </c>
-      <c r="X10" s="11">
+      <c r="X10" s="9">
         <v>0.14486921529175001</v>
       </c>
-      <c r="Y10" s="15">
+      <c r="Y10" s="12">
         <v>0.43636363636363601</v>
       </c>
-      <c r="Z10" s="10">
+      <c r="Z10" s="8">
         <v>0.87951807228915602</v>
       </c>
-      <c r="AA10" s="11">
+      <c r="AA10" s="9">
         <v>0.14807302231237299</v>
       </c>
-      <c r="AB10" s="15">
+      <c r="AB10" s="12">
         <v>0.442424242424242</v>
       </c>
-      <c r="AC10" s="10">
+      <c r="AC10" s="8">
         <v>0.89285714285714202</v>
       </c>
-      <c r="AD10" s="11">
+      <c r="AD10" s="9">
         <v>0.15030060120240399</v>
       </c>
-      <c r="AE10" s="15">
+      <c r="AE10" s="12">
         <v>0.44910179640718501</v>
       </c>
     </row>
@@ -1484,270 +1507,270 @@
       <c r="A11" t="s">
         <v>2</v>
       </c>
-      <c r="B11" s="10">
+      <c r="B11" s="8">
         <v>0.93388429752066104</v>
       </c>
-      <c r="C11" s="11">
+      <c r="C11" s="9">
         <v>0.181380417335473</v>
       </c>
-      <c r="D11" s="15">
+      <c r="D11" s="12">
         <v>0.51038843721770499</v>
       </c>
-      <c r="E11" s="10">
+      <c r="E11" s="8">
         <v>0.96638655462184797</v>
       </c>
-      <c r="F11" s="11">
+      <c r="F11" s="9">
         <v>0.18638573743922199</v>
       </c>
-      <c r="G11" s="15">
+      <c r="G11" s="12">
         <v>0.52607502287282704</v>
       </c>
-      <c r="H11" s="10">
+      <c r="H11" s="8">
         <v>0.93693693693693603</v>
       </c>
-      <c r="I11" s="11">
+      <c r="I11" s="9">
         <v>0.17537942664418199</v>
       </c>
-      <c r="J11" s="15">
+      <c r="J11" s="12">
         <v>0.50144648023143601</v>
       </c>
-      <c r="K11" s="10">
+      <c r="K11" s="8">
         <v>0.94214876033057804</v>
       </c>
-      <c r="L11" s="11">
+      <c r="L11" s="9">
         <v>0.18476499189627199</v>
       </c>
-      <c r="M11" s="15">
+      <c r="M11" s="12">
         <v>0.51771117166212499</v>
       </c>
-      <c r="N11" s="10">
+      <c r="N11" s="8">
         <v>0.92063492063492003</v>
       </c>
-      <c r="O11" s="11">
+      <c r="O11" s="9">
         <v>0.18985270049099801</v>
       </c>
-      <c r="P11" s="15">
+      <c r="P11" s="12">
         <v>0.52017937219730903</v>
       </c>
-      <c r="Q11" s="10">
+      <c r="Q11" s="8">
         <v>0.94</v>
       </c>
-      <c r="R11" s="11">
+      <c r="R11" s="9">
         <v>0.16876122082585199</v>
       </c>
-      <c r="S11" s="15">
+      <c r="S11" s="12">
         <v>0.49111807732497298</v>
       </c>
-      <c r="T11" s="10">
+      <c r="T11" s="8">
         <v>0.93636363636363595</v>
       </c>
-      <c r="U11" s="11">
+      <c r="U11" s="9">
         <v>0.18262411347517701</v>
       </c>
-      <c r="V11" s="15">
+      <c r="V11" s="12">
         <v>0.51294820717131395</v>
       </c>
-      <c r="W11" s="10">
+      <c r="W11" s="8">
         <v>0.93636363636363595</v>
       </c>
-      <c r="X11" s="11">
+      <c r="X11" s="9">
         <v>0.17975567190226799</v>
       </c>
-      <c r="Y11" s="15">
+      <c r="Y11" s="12">
         <v>0.50839091806515302</v>
       </c>
-      <c r="Z11" s="10">
+      <c r="Z11" s="8">
         <v>0.93396226415094297</v>
       </c>
-      <c r="AA11" s="11">
+      <c r="AA11" s="9">
         <v>0.17741935483870899</v>
       </c>
-      <c r="AB11" s="15">
+      <c r="AB11" s="12">
         <v>0.50407331975559999</v>
       </c>
-      <c r="AC11" s="10">
+      <c r="AC11" s="8">
         <v>0.94495412844036697</v>
       </c>
-      <c r="AD11" s="11">
+      <c r="AD11" s="9">
         <v>0.18197879858657201</v>
       </c>
-      <c r="AE11" s="15">
+      <c r="AE11" s="12">
         <v>0.51397205588822303</v>
       </c>
     </row>
     <row r="12" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="B12" s="10"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="15"/>
-      <c r="H12" s="10"/>
-      <c r="I12" s="11"/>
-      <c r="J12" s="15"/>
-      <c r="K12" s="10"/>
-      <c r="L12" s="11"/>
-      <c r="M12" s="15"/>
-      <c r="N12" s="10"/>
-      <c r="O12" s="11"/>
-      <c r="P12" s="15"/>
-      <c r="Q12" s="10"/>
-      <c r="R12" s="11"/>
-      <c r="S12" s="15"/>
-      <c r="T12" s="10"/>
-      <c r="U12" s="11"/>
-      <c r="V12" s="15"/>
-      <c r="W12" s="10"/>
-      <c r="X12" s="11"/>
-      <c r="Y12" s="15"/>
-      <c r="Z12" s="10"/>
-      <c r="AA12" s="11"/>
-      <c r="AB12" s="15"/>
-      <c r="AC12" s="10"/>
-      <c r="AD12" s="11"/>
-      <c r="AE12" s="15"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="12"/>
+      <c r="K12" s="8"/>
+      <c r="L12" s="9"/>
+      <c r="M12" s="12"/>
+      <c r="N12" s="8"/>
+      <c r="O12" s="9"/>
+      <c r="P12" s="12"/>
+      <c r="Q12" s="8"/>
+      <c r="R12" s="9"/>
+      <c r="S12" s="12"/>
+      <c r="T12" s="8"/>
+      <c r="U12" s="9"/>
+      <c r="V12" s="12"/>
+      <c r="W12" s="8"/>
+      <c r="X12" s="9"/>
+      <c r="Y12" s="12"/>
+      <c r="Z12" s="8"/>
+      <c r="AA12" s="9"/>
+      <c r="AB12" s="12"/>
+      <c r="AC12" s="8"/>
+      <c r="AD12" s="9"/>
+      <c r="AE12" s="12"/>
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="5"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="4" t="s">
+      <c r="C13" s="14"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="F13" s="5"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="4" t="s">
+      <c r="F13" s="14"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="I13" s="5"/>
-      <c r="J13" s="12"/>
-      <c r="K13" s="4" t="s">
+      <c r="I13" s="14"/>
+      <c r="J13" s="15"/>
+      <c r="K13" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="L13" s="5"/>
-      <c r="M13" s="12"/>
-      <c r="N13" s="4" t="s">
+      <c r="L13" s="14"/>
+      <c r="M13" s="15"/>
+      <c r="N13" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="O13" s="5"/>
-      <c r="P13" s="12"/>
-      <c r="Q13" s="4" t="s">
+      <c r="O13" s="14"/>
+      <c r="P13" s="15"/>
+      <c r="Q13" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="R13" s="5"/>
-      <c r="S13" s="12"/>
-      <c r="T13" s="4" t="s">
+      <c r="R13" s="14"/>
+      <c r="S13" s="15"/>
+      <c r="T13" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="U13" s="5"/>
-      <c r="V13" s="12"/>
-      <c r="W13" s="4" t="s">
+      <c r="U13" s="14"/>
+      <c r="V13" s="15"/>
+      <c r="W13" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="X13" s="5"/>
-      <c r="Y13" s="12"/>
-      <c r="Z13" s="4" t="s">
+      <c r="X13" s="14"/>
+      <c r="Y13" s="15"/>
+      <c r="Z13" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="AA13" s="5"/>
-      <c r="AB13" s="12"/>
-      <c r="AC13" s="4" t="s">
+      <c r="AA13" s="14"/>
+      <c r="AB13" s="15"/>
+      <c r="AC13" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="AD13" s="5"/>
-      <c r="AE13" s="12"/>
+      <c r="AD13" s="14"/>
+      <c r="AE13" s="15"/>
     </row>
     <row r="14" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="B14" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D14" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F14" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="G14" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="H14" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="I14" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="J14" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="K14" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="L14" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="M14" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="N14" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="O14" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="P14" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q14" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="R14" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="S14" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="T14" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="U14" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="V14" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="W14" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="X14" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="Y14" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="Z14" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="AA14" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="AB14" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="AC14" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="AD14" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="AE14" s="13" t="s">
+      <c r="B14" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G14" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I14" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J14" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="K14" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="L14" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="M14" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="N14" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="O14" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="P14" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q14" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="R14" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="S14" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="T14" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="U14" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="V14" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="W14" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="X14" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y14" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z14" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="AA14" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="AB14" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AC14" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="AD14" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="AE14" s="10" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1755,129 +1778,129 @@
       <c r="A15" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B15" s="8"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="8"/>
-      <c r="I15" s="9"/>
-      <c r="J15" s="14"/>
-      <c r="K15" s="8"/>
-      <c r="L15" s="9"/>
-      <c r="M15" s="14"/>
-      <c r="N15" s="8"/>
-      <c r="O15" s="9"/>
-      <c r="P15" s="14"/>
-      <c r="Q15" s="8"/>
-      <c r="R15" s="9"/>
-      <c r="S15" s="14"/>
-      <c r="T15" s="8"/>
-      <c r="U15" s="9"/>
-      <c r="V15" s="14"/>
-      <c r="W15" s="8"/>
-      <c r="X15" s="9"/>
-      <c r="Y15" s="14"/>
-      <c r="Z15" s="8"/>
-      <c r="AA15" s="9"/>
-      <c r="AB15" s="14"/>
-      <c r="AC15" s="8"/>
-      <c r="AD15" s="9"/>
-      <c r="AE15" s="14"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="7"/>
+      <c r="J15" s="11"/>
+      <c r="K15" s="6"/>
+      <c r="L15" s="7"/>
+      <c r="M15" s="11"/>
+      <c r="N15" s="6"/>
+      <c r="O15" s="7"/>
+      <c r="P15" s="11"/>
+      <c r="Q15" s="6"/>
+      <c r="R15" s="7"/>
+      <c r="S15" s="11"/>
+      <c r="T15" s="6"/>
+      <c r="U15" s="7"/>
+      <c r="V15" s="11"/>
+      <c r="W15" s="6"/>
+      <c r="X15" s="7"/>
+      <c r="Y15" s="11"/>
+      <c r="Z15" s="6"/>
+      <c r="AA15" s="7"/>
+      <c r="AB15" s="11"/>
+      <c r="AC15" s="6"/>
+      <c r="AD15" s="7"/>
+      <c r="AE15" s="11"/>
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>5</v>
       </c>
-      <c r="B16" s="10">
+      <c r="B16" s="8">
         <v>0.761290322580645</v>
       </c>
-      <c r="C16" s="11">
+      <c r="C16" s="9">
         <v>0.103873239436619</v>
       </c>
-      <c r="D16" s="15">
+      <c r="D16" s="12">
         <v>0.33599088838268698</v>
       </c>
-      <c r="E16" s="10">
+      <c r="E16" s="8">
         <v>0.74842767295597401</v>
       </c>
-      <c r="F16" s="11">
+      <c r="F16" s="9">
         <v>0.1</v>
       </c>
-      <c r="G16" s="15">
+      <c r="G16" s="12">
         <v>0.325848849945235</v>
       </c>
-      <c r="H16" s="10">
+      <c r="H16" s="8">
         <v>0.65467625899280502</v>
       </c>
-      <c r="I16" s="11">
+      <c r="I16" s="9">
         <v>9.2292089249492906E-2</v>
       </c>
-      <c r="J16" s="15">
+      <c r="J16" s="12">
         <v>0.29507133592736701</v>
       </c>
-      <c r="K16" s="10">
+      <c r="K16" s="8">
         <v>0.71523178807946997</v>
       </c>
-      <c r="L16" s="11">
+      <c r="L16" s="9">
         <v>9.7385031559963905E-2</v>
       </c>
-      <c r="M16" s="15">
+      <c r="M16" s="12">
         <v>0.31523642732049001</v>
       </c>
-      <c r="N16" s="10">
+      <c r="N16" s="8">
         <v>0.86206896551724099</v>
       </c>
-      <c r="O16" s="11">
+      <c r="O16" s="9">
         <v>0.121527777777777</v>
       </c>
-      <c r="P16" s="15">
+      <c r="P16" s="12">
         <v>0.38854351687388899</v>
       </c>
-      <c r="Q16" s="10">
+      <c r="Q16" s="8">
         <v>0.71917808219178003</v>
       </c>
-      <c r="R16" s="11">
+      <c r="R16" s="9">
         <v>9.8222637979420005E-2</v>
       </c>
-      <c r="S16" s="15">
+      <c r="S16" s="12">
         <v>0.31760435571687801</v>
       </c>
-      <c r="T16" s="10">
+      <c r="T16" s="8">
         <v>0.72108843537414902</v>
       </c>
-      <c r="U16" s="11">
+      <c r="U16" s="9">
         <v>0.100760456273764</v>
       </c>
-      <c r="V16" s="15">
+      <c r="V16" s="12">
         <v>0.32317073170731703</v>
       </c>
-      <c r="W16" s="10">
+      <c r="W16" s="8">
         <v>0.63120567375886505</v>
       </c>
-      <c r="X16" s="11">
+      <c r="X16" s="9">
         <v>9.2323651452282093E-2</v>
       </c>
-      <c r="Y16" s="15">
+      <c r="Y16" s="12">
         <v>0.29123036649214601</v>
       </c>
-      <c r="Z16" s="10">
+      <c r="Z16" s="8">
         <v>0.643356643356643</v>
       </c>
-      <c r="AA16" s="11">
+      <c r="AA16" s="9">
         <v>9.8924731182795697E-2</v>
       </c>
-      <c r="AB16" s="15">
+      <c r="AB16" s="12">
         <v>0.30625832223701699</v>
       </c>
-      <c r="AC16" s="10">
+      <c r="AC16" s="8">
         <v>0.64539007092198497</v>
       </c>
-      <c r="AD16" s="11">
+      <c r="AD16" s="9">
         <v>9.6808510638297804E-2</v>
       </c>
-      <c r="AE16" s="15">
+      <c r="AE16" s="12">
         <v>0.30252659574467999</v>
       </c>
     </row>
@@ -1885,99 +1908,618 @@
       <c r="A17" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="10">
+      <c r="B17" s="8">
         <v>0.81517509727626403</v>
       </c>
-      <c r="C17" s="11">
+      <c r="C17" s="9">
         <v>0.579129232895646</v>
       </c>
-      <c r="D17" s="15">
+      <c r="D17" s="12">
         <v>0.75373268573484398</v>
       </c>
-      <c r="E17" s="10">
+      <c r="E17" s="8">
         <v>0.80434782608695599</v>
       </c>
-      <c r="F17" s="11">
+      <c r="F17" s="9">
         <v>0.56695536309127204</v>
       </c>
-      <c r="G17" s="15">
+      <c r="G17" s="12">
         <v>0.74219431362288502</v>
       </c>
-      <c r="H17" s="10">
+      <c r="H17" s="8">
         <v>0.70315789473684198</v>
       </c>
-      <c r="I17" s="11">
+      <c r="I17" s="9">
         <v>0.54575163398692705</v>
       </c>
-      <c r="J17" s="15">
+      <c r="J17" s="12">
         <v>0.66480891719745205</v>
       </c>
-      <c r="K17" s="10">
+      <c r="K17" s="8">
         <v>0.7734375</v>
       </c>
-      <c r="L17" s="11">
+      <c r="L17" s="9">
         <v>0.56571428571428495</v>
       </c>
-      <c r="M17" s="15">
+      <c r="M17" s="12">
         <v>0.72052401746724803</v>
       </c>
-      <c r="N17" s="10">
+      <c r="N17" s="8">
         <v>0.86271324126726201</v>
       </c>
-      <c r="O17" s="11">
+      <c r="O17" s="9">
         <v>0.57405405405405396</v>
       </c>
-      <c r="P17" s="15">
+      <c r="P17" s="12">
         <v>0.783879539415411</v>
       </c>
-      <c r="Q17" s="10">
+      <c r="Q17" s="8">
         <v>0.75560081466395101</v>
       </c>
-      <c r="R17" s="11">
+      <c r="R17" s="9">
         <v>0.54922279792746098</v>
       </c>
-      <c r="S17" s="15">
+      <c r="S17" s="12">
         <v>0.70278461829892003</v>
       </c>
-      <c r="T17" s="10">
+      <c r="T17" s="8">
         <v>0.74035453597497303</v>
       </c>
-      <c r="U17" s="11">
+      <c r="U17" s="9">
         <v>0.54115853658536495</v>
       </c>
-      <c r="V17" s="15">
+      <c r="V17" s="12">
         <v>0.68958818958818902</v>
       </c>
-      <c r="W17" s="10">
+      <c r="W17" s="8">
         <v>0.70233050847457601</v>
       </c>
-      <c r="X17" s="11">
+      <c r="X17" s="9">
         <v>0.55158069883527405</v>
       </c>
-      <c r="Y17" s="15">
+      <c r="Y17" s="12">
         <v>0.66593009240658896</v>
       </c>
-      <c r="Z17" s="10">
+      <c r="Z17" s="8">
         <v>0.69493278179937901</v>
       </c>
-      <c r="AA17" s="11">
+      <c r="AA17" s="9">
         <v>0.57045840407470205</v>
       </c>
-      <c r="AB17" s="15">
+      <c r="AB17" s="12">
         <v>0.66587395957193796</v>
       </c>
-      <c r="AC17" s="10">
+      <c r="AC17" s="8">
         <v>0.68487394957983105</v>
       </c>
-      <c r="AD17" s="11">
+      <c r="AD17" s="9">
         <v>0.55207451312446998</v>
       </c>
-      <c r="AE17" s="15">
+      <c r="AE17" s="12">
         <v>0.65343756263780295</v>
+      </c>
+    </row>
+    <row r="18" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="B18" s="8"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="12"/>
+      <c r="K18" s="8"/>
+      <c r="L18" s="9"/>
+      <c r="M18" s="12"/>
+      <c r="N18" s="8"/>
+      <c r="O18" s="9"/>
+      <c r="P18" s="12"/>
+      <c r="Q18" s="8"/>
+      <c r="R18" s="9"/>
+      <c r="S18" s="12"/>
+      <c r="T18" s="8"/>
+      <c r="U18" s="9"/>
+      <c r="V18" s="12"/>
+      <c r="W18" s="8"/>
+      <c r="X18" s="9"/>
+      <c r="Y18" s="12"/>
+      <c r="Z18" s="8"/>
+      <c r="AA18" s="9"/>
+      <c r="AB18" s="12"/>
+      <c r="AC18" s="8"/>
+      <c r="AD18" s="9"/>
+      <c r="AE18" s="12"/>
+    </row>
+    <row r="19" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="B19" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" s="14"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="F19" s="14"/>
+      <c r="G19" s="15"/>
+      <c r="H19" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="I19" s="14"/>
+      <c r="J19" s="15"/>
+      <c r="K19" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="L19" s="14"/>
+      <c r="M19" s="15"/>
+      <c r="N19" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="O19" s="14"/>
+      <c r="P19" s="15"/>
+      <c r="Q19" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="R19" s="14"/>
+      <c r="S19" s="15"/>
+      <c r="T19" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="U19" s="14"/>
+      <c r="V19" s="15"/>
+      <c r="W19" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="X19" s="14"/>
+      <c r="Y19" s="15"/>
+      <c r="Z19" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="AA19" s="14"/>
+      <c r="AB19" s="15"/>
+      <c r="AC19" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="AD19" s="14"/>
+      <c r="AE19" s="15"/>
+    </row>
+    <row r="20" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A20" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G20" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="H20" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I20" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J20" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="K20" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="L20" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="M20" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="N20" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="O20" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="P20" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q20" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="R20" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="S20" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="T20" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="U20" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="V20" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="W20" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="X20" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y20" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z20" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="AA20" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="AB20" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AC20" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="AD20" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="AE20" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" s="6"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="11"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="7"/>
+      <c r="J21" s="11"/>
+      <c r="K21" s="6"/>
+      <c r="L21" s="7"/>
+      <c r="M21" s="11"/>
+      <c r="N21" s="6"/>
+      <c r="O21" s="7"/>
+      <c r="P21" s="11"/>
+      <c r="Q21" s="6"/>
+      <c r="R21" s="7"/>
+      <c r="S21" s="11"/>
+      <c r="T21" s="6"/>
+      <c r="U21" s="7"/>
+      <c r="V21" s="11"/>
+      <c r="W21" s="6"/>
+      <c r="X21" s="7"/>
+      <c r="Y21" s="11"/>
+      <c r="Z21" s="6"/>
+      <c r="AA21" s="7"/>
+      <c r="AB21" s="11"/>
+      <c r="AC21" s="6"/>
+      <c r="AD21" s="7"/>
+      <c r="AE21" s="11"/>
+    </row>
+    <row r="22" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A22" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="B22" s="8">
+        <v>0.59202059202059198</v>
+      </c>
+      <c r="C22" s="9">
+        <v>0.43111527647610098</v>
+      </c>
+      <c r="D22" s="12">
+        <v>0.55089820359281405</v>
+      </c>
+      <c r="E22" s="8">
+        <v>0.57907845579078399</v>
+      </c>
+      <c r="F22" s="9">
+        <v>0.42157751586581999</v>
+      </c>
+      <c r="G22" s="12">
+        <v>0.53881807647740398</v>
+      </c>
+      <c r="H22" s="8">
+        <v>0.51539491298527396</v>
+      </c>
+      <c r="I22" s="9">
+        <v>0.41264737406216501</v>
+      </c>
+      <c r="J22" s="12">
+        <v>0.490946187197143</v>
+      </c>
+      <c r="K22" s="8">
+        <v>0.55212355212355202</v>
+      </c>
+      <c r="L22" s="9">
+        <v>0.41976516634050798</v>
+      </c>
+      <c r="M22" s="12">
+        <v>0.51937046004842602</v>
+      </c>
+      <c r="N22" s="8">
+        <v>0.65401785714285698</v>
+      </c>
+      <c r="O22" s="9">
+        <v>0.42711370262390602</v>
+      </c>
+      <c r="P22" s="12">
+        <v>0.59120258272800597</v>
+      </c>
+      <c r="Q22" s="8">
+        <v>0.538258575197889</v>
+      </c>
+      <c r="R22" s="9">
+        <v>0.40356083086053401</v>
+      </c>
+      <c r="S22" s="12">
+        <v>0.50457581004204799</v>
+      </c>
+      <c r="T22" s="8">
+        <v>0.52311756935270703</v>
+      </c>
+      <c r="U22" s="9">
+        <v>0.40243902439024298</v>
+      </c>
+      <c r="V22" s="12">
+        <v>0.49351944167497502</v>
+      </c>
+      <c r="W22" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="X22" s="9">
+        <v>0.41229050279329599</v>
+      </c>
+      <c r="Y22" s="12">
+        <v>0.47959448921237302</v>
+      </c>
+      <c r="Z22" s="8">
+        <v>0.490013315579227</v>
+      </c>
+      <c r="AA22" s="9">
+        <v>0.42494226327944501</v>
+      </c>
+      <c r="AB22" s="12">
+        <v>0.47545219638242803</v>
+      </c>
+      <c r="AC22" s="8">
+        <v>0.48859060402684501</v>
+      </c>
+      <c r="AD22" s="9">
+        <v>0.41037204058624499</v>
+      </c>
+      <c r="AE22" s="12">
+        <v>0.470649081975691</v>
+      </c>
+    </row>
+    <row r="23" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A23" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="B23" s="8">
+        <v>0.64639639639639601</v>
+      </c>
+      <c r="C23" s="9">
+        <v>0.28528827037773302</v>
+      </c>
+      <c r="D23" s="12">
+        <v>0.51581595974119299</v>
+      </c>
+      <c r="E23" s="8">
+        <v>0.64224137931034397</v>
+      </c>
+      <c r="F23" s="9">
+        <v>0.284351145038167</v>
+      </c>
+      <c r="G23" s="12">
+        <v>0.51308539944903497</v>
+      </c>
+      <c r="H23" s="8">
+        <v>0.57783018867924496</v>
+      </c>
+      <c r="I23" s="9">
+        <v>0.277463193657984</v>
+      </c>
+      <c r="J23" s="12">
+        <v>0.474990306320279</v>
+      </c>
+      <c r="K23" s="8">
+        <v>0.62276785714285698</v>
+      </c>
+      <c r="L23" s="9">
+        <v>0.28181818181818102</v>
+      </c>
+      <c r="M23" s="12">
+        <v>0.50143781452192604</v>
+      </c>
+      <c r="N23" s="8">
+        <v>0.71962616822429903</v>
+      </c>
+      <c r="O23" s="9">
+        <v>0.297067901234567</v>
+      </c>
+      <c r="P23" s="12">
+        <v>0.56024447031431901</v>
+      </c>
+      <c r="Q23" s="8">
+        <v>0.59016393442622905</v>
+      </c>
+      <c r="R23" s="9">
+        <v>0.266666666666666</v>
+      </c>
+      <c r="S23" s="12">
+        <v>0.47493403693931402</v>
+      </c>
+      <c r="T23" s="8">
+        <v>0.57981220657276999</v>
+      </c>
+      <c r="U23" s="9">
+        <v>0.26587728740581201</v>
+      </c>
+      <c r="V23" s="12">
+        <v>0.46904671477402199</v>
+      </c>
+      <c r="W23" s="8">
+        <v>0.55581947743467897</v>
+      </c>
+      <c r="X23" s="9">
+        <v>0.27432590855803002</v>
+      </c>
+      <c r="Y23" s="12">
+        <v>0.46117461568781998</v>
+      </c>
+      <c r="Z23" s="8">
+        <v>0.55140186915887801</v>
+      </c>
+      <c r="AA23" s="9">
+        <v>0.28675577156743598</v>
+      </c>
+      <c r="AB23" s="12">
+        <v>0.46548323471400399</v>
+      </c>
+      <c r="AC23" s="8">
+        <v>0.53349282296650702</v>
+      </c>
+      <c r="AD23" s="9">
+        <v>0.26770708283313299</v>
+      </c>
+      <c r="AE23" s="12">
+        <v>0.44510978043912097</v>
+      </c>
+    </row>
+    <row r="24" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A24" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="B24" s="8">
+        <v>0.64333333333333298</v>
+      </c>
+      <c r="C24" s="9">
+        <v>0.18774319066147799</v>
+      </c>
+      <c r="D24" s="12">
+        <v>0.43312387791741402</v>
+      </c>
+      <c r="E24" s="8">
+        <v>0.63862928348909598</v>
+      </c>
+      <c r="F24" s="9">
+        <v>0.190166975881261</v>
+      </c>
+      <c r="G24" s="12">
+        <v>0.433954276037256</v>
+      </c>
+      <c r="H24" s="8">
+        <v>0.57191780821917704</v>
+      </c>
+      <c r="I24" s="9">
+        <v>0.18534961154273</v>
+      </c>
+      <c r="J24" s="12">
+        <v>0.40357660705654902</v>
+      </c>
+      <c r="K24" s="8">
+        <v>0.59283387622149797</v>
+      </c>
+      <c r="L24" s="9">
+        <v>0.18073485600794401</v>
+      </c>
+      <c r="M24" s="12">
+        <v>0.40715883668903702</v>
+      </c>
+      <c r="N24" s="8">
+        <v>0.72340425531914898</v>
+      </c>
+      <c r="O24" s="9">
+        <v>0.20253164556962</v>
+      </c>
+      <c r="P24" s="12">
+        <v>0.47769582016157303</v>
+      </c>
+      <c r="Q24" s="8">
+        <v>0.60967741935483799</v>
+      </c>
+      <c r="R24" s="9">
+        <v>0.191878172588832</v>
+      </c>
+      <c r="S24" s="12">
+        <v>0.42471910112359501</v>
+      </c>
+      <c r="T24" s="8">
+        <v>0.58389261744966403</v>
+      </c>
+      <c r="U24" s="9">
+        <v>0.18143899895724699</v>
+      </c>
+      <c r="V24" s="12">
+        <v>0.40446304044630399</v>
+      </c>
+      <c r="W24" s="8">
+        <v>0.53716216216216195</v>
+      </c>
+      <c r="X24" s="9">
+        <v>0.18317972350230399</v>
+      </c>
+      <c r="Y24" s="12">
+        <v>0.38742690058479501</v>
+      </c>
+      <c r="Z24" s="8">
+        <v>0.54729729729729704</v>
+      </c>
+      <c r="AA24" s="9">
+        <v>0.19239904988123499</v>
+      </c>
+      <c r="AB24" s="12">
+        <v>0.39980256663376101</v>
+      </c>
+      <c r="AC24" s="8">
+        <v>0.53924914675767899</v>
+      </c>
+      <c r="AD24" s="9">
+        <v>0.18436406067677899</v>
+      </c>
+      <c r="AE24" s="12">
+        <v>0.38935436175455801</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="20">
+  <mergeCells count="30">
+    <mergeCell ref="Q19:S19"/>
+    <mergeCell ref="T19:V19"/>
+    <mergeCell ref="W19:Y19"/>
+    <mergeCell ref="Z19:AB19"/>
+    <mergeCell ref="AC19:AE19"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="E19:G19"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="K19:M19"/>
+    <mergeCell ref="N19:P19"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="AC5:AE5"/>
+    <mergeCell ref="Z5:AB5"/>
+    <mergeCell ref="W5:Y5"/>
+    <mergeCell ref="T5:V5"/>
+    <mergeCell ref="Q5:S5"/>
+    <mergeCell ref="N5:P5"/>
+    <mergeCell ref="K5:M5"/>
+    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="E5:G5"/>
     <mergeCell ref="T13:V13"/>
     <mergeCell ref="W13:Y13"/>
     <mergeCell ref="Z13:AB13"/>
@@ -1988,16 +2530,6 @@
     <mergeCell ref="K13:M13"/>
     <mergeCell ref="N13:P13"/>
     <mergeCell ref="Q13:S13"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="AC5:AE5"/>
-    <mergeCell ref="Z5:AB5"/>
-    <mergeCell ref="W5:Y5"/>
-    <mergeCell ref="T5:V5"/>
-    <mergeCell ref="Q5:S5"/>
-    <mergeCell ref="N5:P5"/>
-    <mergeCell ref="K5:M5"/>
-    <mergeCell ref="H5:J5"/>
-    <mergeCell ref="E5:G5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>